<commit_message>
nambah deskripsi dan barang jenis
just in time
</commit_message>
<xml_diff>
--- a/public/files/template.xlsx
+++ b/public/files/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\dvina\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deva satrio\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>id_kategori</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>varian</t>
+  </si>
+  <si>
+    <t>deskripsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,9 +385,10 @@
     <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,6 +409,14 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>